<commit_message>
Organizando o código de exportação
</commit_message>
<xml_diff>
--- a/public/Output_Candidates.xlsx
+++ b/public/Output_Candidates.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -398,232 +398,745 @@
         <v>email</v>
       </c>
       <c r="F1" t="str">
-        <v>additionalInfo</v>
+        <v>candidateNumber</v>
       </c>
       <c r="G1" t="str">
-        <v>candidateStatus</v>
+        <v>createdAt</v>
       </c>
       <c r="H1" t="str">
-        <v>candidateNumber</v>
+        <v>updatedAt</v>
       </c>
       <c r="I1" t="str">
-        <v>createdAt</v>
+        <v>__v</v>
       </c>
       <c r="J1" t="str">
-        <v>updatedAt</v>
+        <v>gender</v>
       </c>
       <c r="K1" t="str">
-        <v>__v</v>
+        <v>relativeName</v>
       </c>
       <c r="L1" t="str">
-        <v>gender</v>
+        <v>birthDate</v>
       </c>
       <c r="M1" t="str">
+        <v>kinship</v>
+      </c>
+      <c r="N1" t="str">
+        <v>phone1</v>
+      </c>
+      <c r="O1" t="str">
+        <v>phone2</v>
+      </c>
+      <c r="P1" t="str">
+        <v>address</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>ifSpecialNecessity</v>
+      </c>
+      <c r="R1" t="str">
+        <v>schooling</v>
+      </c>
+      <c r="S1" t="str">
         <v>school</v>
       </c>
-      <c r="N1" t="str">
+      <c r="T1" t="str">
         <v>kindSchool</v>
       </c>
-      <c r="O1" t="str">
-        <v>ifSpecialNecessity</v>
-      </c>
-      <c r="P1" t="str">
-        <v>phone1</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>kinship</v>
-      </c>
-      <c r="R1" t="str">
-        <v>relativeName</v>
-      </c>
-      <c r="S1" t="str">
-        <v>schooling</v>
-      </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>wayPS</v>
       </c>
-      <c r="U1" t="str">
-        <v>birthDate</v>
-      </c>
       <c r="V1" t="str">
-        <v>additionalAddress</v>
+        <v>_bsontype</v>
       </c>
       <c r="W1" t="str">
-        <v>street</v>
-      </c>
-      <c r="X1" t="str">
-        <v>numberStreet</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>neighborhood</v>
-      </c>
-      <c r="Z1" t="str">
-        <v>city</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>state</v>
-      </c>
-      <c r="AB1" t="str">
-        <v>cep</v>
+        <v>id</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>ko</v>
+        <v>Luís Eduardo</v>
       </c>
       <c r="C2" t="str">
-        <v>lo</v>
+        <v>12221313112121122121211212</v>
       </c>
       <c r="D2" t="str">
-        <v>la</v>
+        <v>12313123131</v>
       </c>
       <c r="E2" t="str">
-        <v>asd</v>
-      </c>
-      <c r="H2">
-        <v>2100026</v>
-      </c>
-      <c r="I2" s="1">
-        <v>44000.44937960648</v>
-      </c>
-      <c r="J2" s="1">
-        <v>44000.44937960648</v>
-      </c>
-      <c r="K2">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F2">
+        <v>2100000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>43999.9644355787</v>
+      </c>
+      <c r="H2" s="1">
+        <v>43999.9644355787</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
+      <c r="J2" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Lalale</v>
+      </c>
       <c r="L2" t="str">
-        <v>feminino</v>
+        <v>20/07/1999</v>
       </c>
       <c r="M2" t="str">
-        <v>christus</v>
+        <v>Pai</v>
       </c>
       <c r="N2" t="str">
-        <v>asd</v>
+        <v>25696969</v>
       </c>
       <c r="O2" t="str">
-        <v>asd</v>
-      </c>
-      <c r="P2" t="str">
-        <v>asd</v>
+        <v>25718901</v>
       </c>
       <c r="Q2" t="str">
-        <v>asd</v>
+        <v>false</v>
       </c>
       <c r="R2" t="str">
-        <v>asd</v>
+        <v>elelellelele</v>
       </c>
       <c r="S2" t="str">
-        <v>asd</v>
+        <v>Martins</v>
       </c>
       <c r="T2" t="str">
-        <v>asd</v>
+        <v>Lale</v>
       </c>
       <c r="U2" t="str">
-        <v>asd</v>
+        <v>Cartomante</v>
       </c>
       <c r="V2" t="str">
-        <v>lulala</v>
-      </c>
-      <c r="W2" t="str">
-        <v>asd</v>
-      </c>
-      <c r="X2">
-        <v>8</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>acula</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>meusovo</v>
-      </c>
-      <c r="AA2" t="str">
-        <v>calango</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>46545</v>
+        <v>ObjectID</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>ka</v>
+        <v>Luiza SONZAAAAAAAAAAaAAA</v>
       </c>
       <c r="C3" t="str">
-        <v>la</v>
+        <v>2121</v>
       </c>
       <c r="D3" t="str">
-        <v>li</v>
+        <v>12313123131</v>
       </c>
       <c r="E3" t="str">
-        <v>asd</v>
-      </c>
-      <c r="H3">
-        <v>2100027</v>
-      </c>
-      <c r="I3" s="1">
-        <v>44000.449379791666</v>
-      </c>
-      <c r="J3" s="1">
-        <v>44000.449379791666</v>
-      </c>
-      <c r="K3">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F3">
+        <v>2100001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43999.96471465278</v>
+      </c>
+      <c r="H3" s="1">
+        <v>43999.96471465278</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
+      <c r="J3" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Lalale</v>
+      </c>
       <c r="L3" t="str">
-        <v>masculino</v>
+        <v>20/07/1999</v>
       </c>
       <c r="M3" t="str">
-        <v>c7s</v>
+        <v>Pai</v>
       </c>
       <c r="N3" t="str">
-        <v>asd</v>
+        <v>25696969</v>
       </c>
       <c r="O3" t="str">
-        <v>asd</v>
-      </c>
-      <c r="P3" t="str">
-        <v>asd</v>
+        <v>25718901</v>
       </c>
       <c r="Q3" t="str">
-        <v>asd</v>
+        <v>false</v>
       </c>
       <c r="R3" t="str">
-        <v>asd</v>
+        <v>elelellelele</v>
       </c>
       <c r="S3" t="str">
-        <v>asd</v>
+        <v>Martins</v>
       </c>
       <c r="T3" t="str">
-        <v>asd</v>
+        <v>Lale</v>
       </c>
       <c r="U3" t="str">
-        <v>asd</v>
+        <v>Cartomante</v>
       </c>
       <c r="V3" t="str">
-        <v>lalalandia</v>
-      </c>
-      <c r="W3" t="str">
-        <v>asd</v>
-      </c>
-      <c r="X3">
-        <v>9</v>
-      </c>
-      <c r="Y3" t="str">
-        <v>ali</v>
-      </c>
-      <c r="Z3" t="str">
-        <v>mamaminha</v>
-      </c>
-      <c r="AA3" t="str">
-        <v>culandia</v>
-      </c>
-      <c r="AB3" t="str">
-        <v>654564</v>
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Luiza SONZAAAAAAAAAAaAAA</v>
+      </c>
+      <c r="C4" t="str">
+        <v>21231311</v>
+      </c>
+      <c r="D4" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E4" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F4">
+        <v>2100002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>43999.96521454861</v>
+      </c>
+      <c r="H4" s="1">
+        <v>43999.96521454861</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L4" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M4" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N4" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O4" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>false</v>
+      </c>
+      <c r="R4" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S4" t="str">
+        <v>Martins</v>
+      </c>
+      <c r="T4" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U4" t="str">
+        <v>Cartomante</v>
+      </c>
+      <c r="V4" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>Luís Eduardo</v>
+      </c>
+      <c r="C5" t="str">
+        <v>212321211311</v>
+      </c>
+      <c r="D5" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E5" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F5">
+        <v>2100003</v>
+      </c>
+      <c r="G5" s="1">
+        <v>43999.97054806713</v>
+      </c>
+      <c r="H5" s="1">
+        <v>43999.97054806713</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L5" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M5" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N5" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O5" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>false</v>
+      </c>
+      <c r="R5" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S5" t="str">
+        <v>Martins</v>
+      </c>
+      <c r="T5" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U5" t="str">
+        <v>Cartomante</v>
+      </c>
+      <c r="V5" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>Luiza SONZAasasaasasaAAAAAAAAAaAAA</v>
+      </c>
+      <c r="C6" t="str">
+        <v>21232211211311</v>
+      </c>
+      <c r="D6" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E6" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F6">
+        <v>2100004</v>
+      </c>
+      <c r="G6" s="1">
+        <v>43999.973579108795</v>
+      </c>
+      <c r="H6" s="1">
+        <v>43999.973579108795</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L6" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M6" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N6" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O6" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>false</v>
+      </c>
+      <c r="R6" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S6" t="str">
+        <v>Martins</v>
+      </c>
+      <c r="T6" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U6" t="str">
+        <v>Cartomante</v>
+      </c>
+      <c r="V6" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Luiza SONZAasasaasasaAAAAAAAAAaAAA</v>
+      </c>
+      <c r="C7" t="str">
+        <v>212322112121211311</v>
+      </c>
+      <c r="D7" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E7" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F7">
+        <v>2100005</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44000.09240047454</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44000.09240047454</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L7" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M7" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N7" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O7" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>false</v>
+      </c>
+      <c r="R7" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S7" t="str">
+        <v>Martins</v>
+      </c>
+      <c r="T7" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U7" t="str">
+        <v>Cartomante</v>
+      </c>
+      <c r="V7" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Luís Eduardo</v>
+      </c>
+      <c r="C8" t="str">
+        <v>212322122112121211311</v>
+      </c>
+      <c r="D8" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E8" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F8">
+        <v>2100006</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44000.110435717594</v>
+      </c>
+      <c r="H8" s="1">
+        <v>44000.143256400464</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L8" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M8" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N8" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O8" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>false</v>
+      </c>
+      <c r="R8" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S8" t="str">
+        <v>Maartinzão</v>
+      </c>
+      <c r="T8" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U8" t="str">
+        <v>Cararadstomante</v>
+      </c>
+      <c r="V8" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Luasaís Eduardo</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2123222121122112121211311</v>
+      </c>
+      <c r="D9" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E9" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F9">
+        <v>2100007</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44000.153003761574</v>
+      </c>
+      <c r="H9" s="1">
+        <v>44000.153003761574</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K9" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L9" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N9" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O9" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>false</v>
+      </c>
+      <c r="R9" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S9" t="str">
+        <v>Maartinzão</v>
+      </c>
+      <c r="T9" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U9" t="str">
+        <v>Cararadstomante</v>
+      </c>
+      <c r="V9" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>Luasaís Eduardo</v>
+      </c>
+      <c r="C10" t="str">
+        <v>21232221211231312112121211311</v>
+      </c>
+      <c r="D10" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E10" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F10">
+        <v>2100008</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44000.153451666665</v>
+      </c>
+      <c r="H10" s="1">
+        <v>44000.153451666665</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L10" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N10" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O10" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>false</v>
+      </c>
+      <c r="R10" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S10" t="str">
+        <v>Maartinzão</v>
+      </c>
+      <c r="T10" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U10" t="str">
+        <v>Cararadstomante</v>
+      </c>
+      <c r="V10" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>Luasaís Eduardo</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2123222121131312231312112121211311</v>
+      </c>
+      <c r="D11" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E11" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F11">
+        <v>2100009</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44000.155725613426</v>
+      </c>
+      <c r="H11" s="1">
+        <v>44000.155725613426</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K11" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L11" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M11" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N11" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O11" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>false</v>
+      </c>
+      <c r="R11" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S11" t="str">
+        <v>Maartinzão</v>
+      </c>
+      <c r="T11" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U11" t="str">
+        <v>Cararadstomante</v>
+      </c>
+      <c r="V11" t="str">
+        <v>ObjectID</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>Luasaís Eduardo</v>
+      </c>
+      <c r="C12" t="str">
+        <v>21232221211313122313121121213121211311</v>
+      </c>
+      <c r="D12" t="str">
+        <v>12313123131</v>
+      </c>
+      <c r="E12" t="str">
+        <v>lalalal@gmail.com</v>
+      </c>
+      <c r="F12">
+        <v>2100010</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44000.58728846065</v>
+      </c>
+      <c r="H12" s="1">
+        <v>44000.58728846065</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Man</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Lalale</v>
+      </c>
+      <c r="L12" t="str">
+        <v>20/07/1999</v>
+      </c>
+      <c r="M12" t="str">
+        <v>Pai</v>
+      </c>
+      <c r="N12" t="str">
+        <v>25696969</v>
+      </c>
+      <c r="O12" t="str">
+        <v>25718901</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>false</v>
+      </c>
+      <c r="R12" t="str">
+        <v>elelellelele</v>
+      </c>
+      <c r="S12" t="str">
+        <v>Maartinzão</v>
+      </c>
+      <c r="T12" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="U12" t="str">
+        <v>Cararadstomante</v>
+      </c>
+      <c r="V12" t="str">
+        <v>ObjectID</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>